<commit_message>
fix: VR data were not recorded due to selection manager only works with mouth click. temporarily fixed this issue by moving data recording to the PDStateManager
</commit_message>
<xml_diff>
--- a/InteractiveLab/subject sheet.xlsx
+++ b/InteractiveLab/subject sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\InteractiveLabPOC\InteractiveLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE91B5E-AEAF-4CAB-B383-0DB72E30AB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AF7D9C-5E99-4D05-BE54-635FC84454EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B53095F0-0CA3-47DD-8DFC-30AAFD0743B8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>par id</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>screen</t>
+  </si>
+  <si>
+    <t>BA</t>
   </si>
 </sst>
 </file>
@@ -391,138 +394,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9367AA3B-033F-4ED0-9BB0-CE6E39CDE760}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>20250107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
data collection par 2 session 1 screen
</commit_message>
<xml_diff>
--- a/InteractiveLab/subject sheet.xlsx
+++ b/InteractiveLab/subject sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\InteractiveLabPOC\InteractiveLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AF7D9C-5E99-4D05-BE54-635FC84454EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4C799C-3F1C-4D53-A55B-12F3DD345C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B53095F0-0CA3-47DD-8DFC-30AAFD0743B8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
   <si>
     <t>par id</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>BA</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -98,9 +101,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -138,7 +141,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -244,7 +247,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -386,7 +389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -397,7 +400,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,6 +443,12 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>20250107</v>
+      </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
data collection: participant 3 session 1 screen - headset disconnected at around the end of part 1 had to restart. need to stitch the data together.
</commit_message>
<xml_diff>
--- a/InteractiveLab/subject sheet.xlsx
+++ b/InteractiveLab/subject sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\InteractiveLabPOC\InteractiveLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4C799C-3F1C-4D53-A55B-12F3DD345C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66747F2D-1E94-46D4-97BB-99EE23E6E972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B53095F0-0CA3-47DD-8DFC-30AAFD0743B8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>par id</t>
   </si>
@@ -45,7 +45,16 @@
     <t>BA</t>
   </si>
   <si>
-    <t>S</t>
+    <t>SY</t>
+  </si>
+  <si>
+    <t>NZ</t>
+  </si>
+  <si>
+    <t>Year since course</t>
+  </si>
+  <si>
+    <t>DT</t>
   </si>
 </sst>
 </file>
@@ -397,32 +406,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9367AA3B-033F-4ED0-9BB0-CE6E39CDE760}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -430,16 +445,19 @@
         <v>5</v>
       </c>
       <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
         <v>20250107</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -447,100 +465,118 @@
         <v>6</v>
       </c>
       <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
         <v>20250107</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>20250108</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>20250108</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
data collection par 1 session 2 screen; par 4 session 1 screen
</commit_message>
<xml_diff>
--- a/InteractiveLab/subject sheet.xlsx
+++ b/InteractiveLab/subject sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\InteractiveLabPOC\InteractiveLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66747F2D-1E94-46D4-97BB-99EE23E6E972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1ABC6F-5EA0-472D-A530-80899F357C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B53095F0-0CA3-47DD-8DFC-30AAFD0743B8}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{B53095F0-0CA3-47DD-8DFC-30AAFD0743B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>par id</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>DT</t>
+  </si>
+  <si>
+    <t>TA for the lab course</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9367AA3B-033F-4ED0-9BB0-CE6E39CDE760}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,7 +420,7 @@
     <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,19 +428,19 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -447,17 +450,20 @@
       <c r="C2">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2">
         <v>20250107</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>20250108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -467,17 +473,17 @@
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
         <v>20250107</v>
       </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -487,96 +493,102 @@
       <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4">
         <v>20250108</v>
       </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="D5">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5">
         <v>20250108</v>
       </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
data collection par 1 session 2 VR
</commit_message>
<xml_diff>
--- a/InteractiveLab/subject sheet.xlsx
+++ b/InteractiveLab/subject sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\InteractiveLabPOC\InteractiveLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1ABC6F-5EA0-472D-A530-80899F357C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBACD01-DAB1-4707-BBDC-B0C1DFFF7C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{B53095F0-0CA3-47DD-8DFC-30AAFD0743B8}"/>
   </bookViews>
@@ -412,7 +412,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,6 +522,9 @@
       <c r="F5" t="s">
         <v>3</v>
       </c>
+      <c r="G5">
+        <v>20250109</v>
+      </c>
       <c r="H5" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
data collection participant 2 session 2 VR
</commit_message>
<xml_diff>
--- a/InteractiveLab/subject sheet.xlsx
+++ b/InteractiveLab/subject sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\InteractiveLabPOC\InteractiveLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBACD01-DAB1-4707-BBDC-B0C1DFFF7C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC0A22B-C7A0-4C40-A568-81B5E835D252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{B53095F0-0CA3-47DD-8DFC-30AAFD0743B8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B53095F0-0CA3-47DD-8DFC-30AAFD0743B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>par id</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>TA for the lab course</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>VW</t>
   </si>
 </sst>
 </file>
@@ -93,8 +99,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,189 +424,265 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.77734375" customWidth="1"/>
     <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>20250107</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>20250108</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>20250107</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G3" s="1">
+        <v>20250109</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>20250108</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>20250108</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>20250109</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
data collection participant 5 session 1 VR
</commit_message>
<xml_diff>
--- a/InteractiveLab/subject sheet.xlsx
+++ b/InteractiveLab/subject sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\InteractiveLabPOC\InteractiveLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC0A22B-C7A0-4C40-A568-81B5E835D252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EAAD89-8155-401B-B539-05C8805F8500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B53095F0-0CA3-47DD-8DFC-30AAFD0743B8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>par id</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>VW</t>
+  </si>
+  <si>
+    <t>TA for the lab course (2023, 2024)</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,15 +563,22 @@
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>20250109</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1"/>
+      <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">

</xml_diff>

<commit_message>
data collection participant 3 session 2 screen
</commit_message>
<xml_diff>
--- a/InteractiveLab/subject sheet.xlsx
+++ b/InteractiveLab/subject sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\InteractiveLabPOC\InteractiveLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EAAD89-8155-401B-B539-05C8805F8500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA735D4-2DAB-441D-AF46-08576FCB134F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B53095F0-0CA3-47DD-8DFC-30AAFD0743B8}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,7 +528,9 @@
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1">
+        <v>20250109</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">

</xml_diff>

<commit_message>
data collection participant 5 session 2 screen
</commit_message>
<xml_diff>
--- a/InteractiveLab/subject sheet.xlsx
+++ b/InteractiveLab/subject sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\InteractiveLabPOC\InteractiveLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA735D4-2DAB-441D-AF46-08576FCB134F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1BF287-D7B6-4FE5-99D4-7125326D4E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B53095F0-0CA3-47DD-8DFC-30AAFD0743B8}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{B53095F0-0CA3-47DD-8DFC-30AAFD0743B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>par id</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>TA for the lab course (2023, 2024)</t>
+  </si>
+  <si>
+    <t>CQ</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,7 +580,9 @@
       <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1">
+        <v>20240110</v>
+      </c>
       <c r="H6" s="2" t="s">
         <v>13</v>
       </c>
@@ -586,7 +591,9 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
         <v>4</v>

</xml_diff>